<commit_message>
create test file for move Y, clean project archi
</commit_message>
<xml_diff>
--- a/NOUVEAU_Projet_Jukebox.xlsx
+++ b/NOUVEAU_Projet_Jukebox.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Raspberry\Jukebox-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0627CE74-EA47-4F3C-915E-E6981AA42FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A41D89F-04FA-4FD1-8D72-31A00E4C76EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cahier des charges" sheetId="1" r:id="rId1"/>
-    <sheet name="Tâches Raspberry Mécanique" sheetId="6" r:id="rId2"/>
-    <sheet name="Electroaimant" sheetId="9" r:id="rId3"/>
-    <sheet name="Tâches app" sheetId="3" r:id="rId4"/>
-    <sheet name="Matériel" sheetId="8" r:id="rId5"/>
-    <sheet name="Questions" sheetId="5" r:id="rId6"/>
-    <sheet name="Techno" sheetId="4" r:id="rId7"/>
+    <sheet name="Raspberry" sheetId="10" r:id="rId2"/>
+    <sheet name="Tâches Raspberry Mécanique" sheetId="6" r:id="rId3"/>
+    <sheet name="Electroaimant" sheetId="9" r:id="rId4"/>
+    <sheet name="Tâches app" sheetId="3" r:id="rId5"/>
+    <sheet name="Matériel" sheetId="8" r:id="rId6"/>
+    <sheet name="Questions" sheetId="5" r:id="rId7"/>
+    <sheet name="Techno" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="278">
   <si>
     <t>Partie App</t>
   </si>
@@ -753,13 +754,290 @@
   </si>
   <si>
     <t>5V</t>
+  </si>
+  <si>
+    <t>Installation lib python3 (pip3 install)</t>
+  </si>
+  <si>
+    <t>Executer app python (python3 app.py)</t>
+  </si>
+  <si>
+    <t>Install pip3</t>
+  </si>
+  <si>
+    <t>apt install python3-pip</t>
+  </si>
+  <si>
+    <t>command</t>
+  </si>
+  <si>
+    <t>Raspberry Pi imager</t>
+  </si>
+  <si>
+    <t>Copy files backend</t>
+  </si>
+  <si>
+    <t>Branchez votre clé USB sur votre ordinateur.</t>
+  </si>
+  <si>
+    <t>Ouvrez un terminal.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Identifiez le nom de périphérique de votre clé USB. Vous pouvez le faire en utilisant la commande </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>lsblk</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">. Par exemple, votre clé USB pourrait être identifiée comme </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>/dev/sdb</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Montez la clé USB. Si elle n'est pas déjà montée automatiquement, vous pouvez le faire en utilisant la commande </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>sudo mount /dev/sdX /mnt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, où </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>/dev/sdX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> est le nom de périphérique de votre clé USB.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Accédez au répertoire où vous souhaitez copier les fichiers. Par exemple, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>cd /home/charl/jukebox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Copiez les fichiers de la clé USB vers ce répertoire en utilisant la commande </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>sudo cp -r /mnt/* .</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Cette commande copiera tous les fichiers et dossiers de la clé USB vers le dossier </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>/home/charl/jukebox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Une fois la copie terminée, vous pouvez démonter la clé USB en utilisant la commande </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>sudo umount /mnt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Débranchez votre clé USB en toute sécurité.</t>
+  </si>
+  <si>
+    <t>Install requirements</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Setup raspOs lite</t>
+  </si>
+  <si>
+    <t>pip3 install -r requirements</t>
+  </si>
+  <si>
+    <t>Test exec python app</t>
+  </si>
+  <si>
+    <t>python3 app.py</t>
+  </si>
+  <si>
+    <t>Create systemctl file</t>
+  </si>
+  <si>
+    <t>[Unit]</t>
+  </si>
+  <si>
+    <t>Description=Flask App</t>
+  </si>
+  <si>
+    <t>After=network.target</t>
+  </si>
+  <si>
+    <t>[Service]</t>
+  </si>
+  <si>
+    <t>User=root</t>
+  </si>
+  <si>
+    <t>Group=root</t>
+  </si>
+  <si>
+    <t>WorkingDirectory=/home/charl/jukebox/backend</t>
+  </si>
+  <si>
+    <t>ExecStart=/usr/bin/python3 /home/charl/jukebox/backend/app.py</t>
+  </si>
+  <si>
+    <t>Restart=always</t>
+  </si>
+  <si>
+    <t>[Install]</t>
+  </si>
+  <si>
+    <t>WantedBy=multi-user.target</t>
+  </si>
+  <si>
+    <t>nano /etc/systemd/system/jukebox.service</t>
+  </si>
+  <si>
+    <t>sudo systemctl daemon-reload</t>
+  </si>
+  <si>
+    <t>sudo systemctl start jukebox</t>
+  </si>
+  <si>
+    <t>sudo systemctl status jukebox</t>
+  </si>
+  <si>
+    <t>sudo systemctl enable jukebox</t>
+  </si>
+  <si>
+    <t>ssh -L 5025:127.0.0.1:5025 charl@169.254.76.59</t>
+  </si>
+  <si>
+    <t>SSH connection with access to python app</t>
+  </si>
+  <si>
+    <t>Sauvegarde auto des données en quittant un champ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,8 +1102,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3C963C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -856,8 +1153,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -885,11 +1188,140 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -1021,6 +1453,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,8 +1649,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3E6AA73-8D41-471D-8991-A1E50578AF6D}" name="Tableau6" displayName="Tableau6" ref="C4:H60" totalsRowShown="0" dataDxfId="27">
-  <autoFilter ref="C4:H60" xr:uid="{A3E6AA73-8D41-471D-8991-A1E50578AF6D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3E6AA73-8D41-471D-8991-A1E50578AF6D}" name="Tableau6" displayName="Tableau6" ref="C4:H64" totalsRowShown="0" dataDxfId="27">
+  <autoFilter ref="C4:H64" xr:uid="{A3E6AA73-8D41-471D-8991-A1E50578AF6D}"/>
   <tableColumns count="6">
     <tableColumn id="11" xr3:uid="{C803E650-A104-4673-B4D1-0C8B2F2CCE65}" name="N° CDC" dataDxfId="26"/>
     <tableColumn id="1" xr3:uid="{307B7E50-701C-4944-A12F-CBFB3F3AB728}" name="Tâche" dataDxfId="25"/>
@@ -1196,8 +1664,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5AC7E31C-C286-4500-9C4E-317003642B50}" name="Tableau25" displayName="Tableau25" ref="C5:E30" totalsRowShown="0" dataDxfId="20">
-  <autoFilter ref="C5:E30" xr:uid="{5AC7E31C-C286-4500-9C4E-317003642B50}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5AC7E31C-C286-4500-9C4E-317003642B50}" name="Tableau25" displayName="Tableau25" ref="C5:E32" totalsRowShown="0" dataDxfId="20">
+  <autoFilter ref="C5:E32" xr:uid="{5AC7E31C-C286-4500-9C4E-317003642B50}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{007B7E2B-3653-49E0-B0FC-44D1A302EB8B}" name="Partie App Frontend" dataDxfId="19"/>
     <tableColumn id="2" xr3:uid="{FFBF547D-A030-4B3C-A989-A377D5A6906B}" name="Priorité" dataDxfId="18"/>
@@ -1546,8 +2014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:F84"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2130,11 +2598,231 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D27CBA-C962-412E-89DF-8B48ECA28584}">
+  <dimension ref="B1:C32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="39.5546875" customWidth="1"/>
+    <col min="3" max="3" width="102.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="57" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="53" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="59" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B5" s="49" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B6" s="51"/>
+      <c r="C6" s="52" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B7" s="51"/>
+      <c r="C7" s="52" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B8" s="51"/>
+      <c r="C8" s="52" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B9" s="51"/>
+      <c r="C9" s="52" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B10" s="51"/>
+      <c r="C10" s="52" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B11" s="51"/>
+      <c r="C11" s="52" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B12" s="53"/>
+      <c r="C12" s="54" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B13" s="59" t="s">
+        <v>252</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B14" s="48" t="s">
+        <v>256</v>
+      </c>
+      <c r="C14" s="55" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="62" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="63" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="64"/>
+      <c r="C16" s="65" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="64"/>
+      <c r="C17" s="65" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="64"/>
+      <c r="C18" s="65" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="64"/>
+      <c r="C19" s="65" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="64"/>
+      <c r="C20" s="65" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="64"/>
+      <c r="C21" s="65" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="64"/>
+      <c r="C22" s="65" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="64"/>
+      <c r="C23" s="65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="64"/>
+      <c r="C24" s="65" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="64"/>
+      <c r="C25" s="65" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="64"/>
+      <c r="C26" s="65" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="64"/>
+      <c r="C27" s="65"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="64"/>
+      <c r="C28" s="65" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="64"/>
+      <c r="C29" s="65" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="64"/>
+      <c r="C30" s="65" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31" s="64"/>
+      <c r="C31" s="67" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="48" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFFA633-1D9B-45BC-A35F-10D4292CF64D}">
-  <dimension ref="C4:H60"/>
+  <dimension ref="C4:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2256,7 +2944,7 @@
         <v>228</v>
       </c>
       <c r="F11" s="19"/>
-      <c r="G11" s="45"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="19"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
@@ -2276,7 +2964,7 @@
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
-      <c r="G13" s="45"/>
+      <c r="G13" s="69"/>
       <c r="H13" s="19"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
@@ -2286,7 +2974,7 @@
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
-      <c r="G14" s="45"/>
+      <c r="G14" s="69"/>
       <c r="H14" s="19"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
@@ -2298,7 +2986,7 @@
         <v>230</v>
       </c>
       <c r="F15" s="19"/>
-      <c r="G15" s="45"/>
+      <c r="G15" s="69"/>
       <c r="H15" s="19"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
@@ -2364,7 +3052,7 @@
       </c>
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
-      <c r="G21" s="45"/>
+      <c r="G21" s="68"/>
       <c r="H21" s="19"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.3">
@@ -2376,7 +3064,7 @@
       </c>
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
-      <c r="G22" s="45"/>
+      <c r="G22" s="68"/>
       <c r="H22" s="19"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.3">
@@ -2384,11 +3072,11 @@
         <v>156</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
-      <c r="G23" s="45"/>
+      <c r="G23" s="68"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.3">
@@ -2396,11 +3084,11 @@
         <v>156</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>190</v>
+        <v>238</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
-      <c r="G24" s="45"/>
+      <c r="G24" s="68"/>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.3">
@@ -2408,27 +3096,23 @@
       <c r="D25" s="19"/>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
-      <c r="G25" s="45"/>
+      <c r="G25" s="68"/>
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C26" s="42">
-        <v>3</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>132</v>
+      <c r="C26" s="19"/>
+      <c r="D26" s="44" t="s">
+        <v>191</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
-      <c r="G26" s="45"/>
+      <c r="G26" s="68"/>
       <c r="H26" s="19"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C27" s="19" t="s">
-        <v>157</v>
-      </c>
+      <c r="C27" s="19"/>
       <c r="D27" s="44" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
@@ -2436,35 +3120,27 @@
       <c r="H27" s="19"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C28" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="D28" s="44" t="s">
-        <v>215</v>
-      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="45"/>
       <c r="H28" s="19"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C29" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="D29" s="44" t="s">
-        <v>198</v>
-      </c>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="45"/>
       <c r="H29" s="19"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C30" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D30" s="44" t="s">
-        <v>196</v>
+      <c r="C30" s="42">
+        <v>3</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>132</v>
       </c>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
@@ -2473,50 +3149,46 @@
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D31" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>201</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="45"/>
       <c r="H31" s="19"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" s="19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>202</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>200</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="45"/>
       <c r="H32" s="19"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="C33" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>198</v>
+      </c>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
       <c r="G33" s="45"/>
       <c r="H33" s="19"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C34" s="42">
-        <v>4</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>133</v>
+      <c r="C34" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" s="44" t="s">
+        <v>196</v>
       </c>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
@@ -2525,46 +3197,50 @@
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C35" s="19" t="s">
-        <v>158</v>
-      </c>
-      <c r="D35" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
+        <v>172</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>201</v>
+      </c>
       <c r="G35" s="45"/>
       <c r="H35" s="19"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C36" s="19" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="D36" s="44" t="s">
-        <v>211</v>
-      </c>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+        <v>202</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>200</v>
+      </c>
       <c r="G36" s="45"/>
       <c r="H36" s="19"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C37" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>214</v>
-      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="45"/>
       <c r="H37" s="19"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C38" s="19"/>
-      <c r="D38" s="44" t="s">
-        <v>212</v>
+      <c r="C38" s="42">
+        <v>4</v>
+      </c>
+      <c r="D38" s="42" t="s">
+        <v>133</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
@@ -2573,10 +3249,10 @@
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C39" s="19" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D39" s="44" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
@@ -2584,45 +3260,59 @@
       <c r="H39" s="19"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
+      <c r="C40" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D40" s="44" t="s">
+        <v>211</v>
+      </c>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="45"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
+      <c r="C41" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>214</v>
+      </c>
       <c r="F41" s="19"/>
       <c r="G41" s="45"/>
       <c r="H41" s="19"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
+      <c r="D42" s="44" t="s">
+        <v>212</v>
+      </c>
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+      <c r="G42" s="45"/>
       <c r="H42" s="19"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
+      <c r="C43" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D43" s="44" t="s">
+        <v>213</v>
+      </c>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
+      <c r="G43" s="45"/>
       <c r="H43" s="19"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C44" s="19"/>
-      <c r="D44" s="19" t="s">
-        <v>105</v>
-      </c>
+      <c r="D44" s="19"/>
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
+      <c r="G44" s="45"/>
       <c r="H44" s="19"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.3">
@@ -2630,7 +3320,7 @@
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
+      <c r="G45" s="45"/>
       <c r="H45" s="19"/>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.3">
@@ -2651,7 +3341,9 @@
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
       <c r="G48" s="19"/>
@@ -2752,6 +3444,38 @@
       <c r="F60" s="19"/>
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2762,7 +3486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8829FC73-E452-4EC9-82EF-B3D3B340C9E7}">
   <dimension ref="B3:C5"/>
   <sheetViews>
@@ -2801,12 +3525,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0ABEB14-C33D-400C-8375-6EF8D376F2C7}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3010,7 +3734,18 @@
       </c>
       <c r="E30" s="21"/>
     </row>
-    <row r="32" spans="3:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
     <row r="33" spans="3:4" ht="45" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="3:4" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="16" t="s">
@@ -3084,7 +3819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB62929-51DD-4306-8C74-3439DC3182AE}">
   <dimension ref="C4:K30"/>
   <sheetViews>
@@ -3548,7 +4283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7A911E-13EF-4BF1-843F-EE228A4C4563}">
   <dimension ref="C2:D11"/>
   <sheetViews>
@@ -3622,7 +4357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4BC952-7BE6-42AA-96C8-BA2D5DB26387}">
   <dimension ref="B3:C7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add/edit files to controller step motors X and Y, servomotor Z and electro magnet. Starting setup stepmachine. Add model 3d for interruptors
</commit_message>
<xml_diff>
--- a/NOUVEAU_Projet_Jukebox.xlsx
+++ b/NOUVEAU_Projet_Jukebox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Raspberry\Jukebox-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3036119-5338-4A6C-96FB-008D025C2B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1F4B3A-A977-47F3-92F4-A7D37587300B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taches en cours" sheetId="12" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="373">
   <si>
     <t>Partie App</t>
   </si>
@@ -663,9 +663,6 @@
   </si>
   <si>
     <t>Trouver des équivalnt qui existent</t>
-  </si>
-  <si>
-    <t>Une fois la strucutre sur, je peux commencer à la créer, et tester éléc en même temps</t>
   </si>
   <si>
     <t>Fixer tige filetée sur le moteur</t>
@@ -1059,9 +1056,6 @@
     <t>=&gt; machine a état</t>
   </si>
   <si>
-    <t>Tester electroaimant sur raspberry</t>
-  </si>
-  <si>
     <t>Nacelle déplacement en X</t>
   </si>
   <si>
@@ -1071,18 +1065,6 @@
     <t>=&gt; Comment enlever les aimants facilement des cds, si besoin</t>
   </si>
   <si>
-    <t>Attend détection interrupteurs</t>
-  </si>
-  <si>
-    <t>Puis va en haut a droite, en comptant le nombre de step pour y arriver (en X et en Y)</t>
-  </si>
-  <si>
-    <t>Sauvegarder les steps</t>
-  </si>
-  <si>
-    <t>Déduire l'emplacement du lecteur, et des CD, avec le nombre de steps</t>
-  </si>
-  <si>
     <t>CD en place ?</t>
   </si>
   <si>
@@ -1110,31 +1092,232 @@
     <t>MoveY(, "cw") jusqu'à la limite (interrupteur se déclenche)</t>
   </si>
   <si>
-    <t>Préparer une variable stepX, à 0</t>
-  </si>
-  <si>
-    <t>MoveX(, "ccw") jusqu'à la limite (interrupteur se déclenche), et incrémente stepX</t>
-  </si>
-  <si>
     <t>Sauvegarder le nombre de step pour aller de droite à gauche</t>
   </si>
   <si>
-    <t>Préparer une variable stepY, à 0</t>
-  </si>
-  <si>
-    <t>MoveY(, "ccw") jusqu'à la limite (interrupteur se déclenche), et incrémente stepY</t>
-  </si>
-  <si>
     <t>Sauvegarder le nombre de step pour aller de bas en haut</t>
   </si>
   <si>
-    <t>branchements OK ?</t>
-  </si>
-  <si>
-    <t>Différentes fonctions</t>
-  </si>
-  <si>
     <t>Trou pour fixer tige en Y + roulement, puis tester</t>
+  </si>
+  <si>
+    <t>Une fois la structure sur, je peux commencer à la créer, et tester éléc en même temps</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ça avec un truc en dezsous pour coulisser sur le bois</t>
+  </si>
+  <si>
+    <t>Utiisation du clavier, 4 flèches de direction</t>
+  </si>
+  <si>
+    <t>Déplacement de l'aimant jusqu'en face des cds</t>
+  </si>
+  <si>
+    <t>Setup positions manuellement des coordonnées</t>
+  </si>
+  <si>
+    <t>Compter le nb de step pour aller à un emplacement</t>
+  </si>
+  <si>
+    <t>Sauvegarder cette valeur dans un json ?</t>
+  </si>
+  <si>
+    <t>Sauvegarder le JSON des données de l'app hors du dossier, pour ne pas ecraser a chaque maj ?</t>
+  </si>
+  <si>
+    <t>GoToOrigin</t>
+  </si>
+  <si>
+    <t>Permet de replacer la jukebox en bas a gauche</t>
+  </si>
+  <si>
+    <t>Prochaine état : GoToOrigin</t>
+  </si>
+  <si>
+    <t>Prochain état : Wait</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>Attente d'un action</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>maxStepX</t>
+  </si>
+  <si>
+    <t>maxStepY</t>
+  </si>
+  <si>
+    <t>Préparer une variable maxStepX, à 0</t>
+  </si>
+  <si>
+    <t>MoveX(, "ccw") jusqu'à la limite (interrupteur se déclenche), et incrémente maxStepX</t>
+  </si>
+  <si>
+    <t>Préparer une variable maxStepY, à 0</t>
+  </si>
+  <si>
+    <t>MoveY(, "ccw") jusqu'à la limite (interrupteur se déclenche), et incrémente maxStepY</t>
+  </si>
+  <si>
+    <t>locationsPos</t>
+  </si>
+  <si>
+    <t>Explocation</t>
+  </si>
+  <si>
+    <t>JSON, contient les 9 position possible (dont 5 pos du lecteur), avec nb de step pour aller a chaque, en partant de l'origin</t>
+  </si>
+  <si>
+    <t>Int, nb de step pour aller d'un côté à l'autre</t>
+  </si>
+  <si>
+    <t>On avance en Z pour se rapprocher du lecteur</t>
+  </si>
+  <si>
+    <t>on active l'electroaimant</t>
+  </si>
+  <si>
+    <t>on recule en Z</t>
+  </si>
+  <si>
+    <t>On avance en Z pour se rapprocher de la position</t>
+  </si>
+  <si>
+    <t>On desactive l'electroaimant</t>
+  </si>
+  <si>
+    <t>Prochain état : GoToPos</t>
+  </si>
+  <si>
+    <t>Int, contient l'id du cCD qu'on souhaite positionner</t>
+  </si>
+  <si>
+    <t>NewAction</t>
+  </si>
+  <si>
+    <t>Play</t>
+  </si>
+  <si>
+    <t>Pause</t>
+  </si>
+  <si>
+    <t>Stop</t>
+  </si>
+  <si>
+    <t>playerActions</t>
+  </si>
+  <si>
+    <t>Liste des différentes action : play, pause, stop</t>
+  </si>
+  <si>
+    <t>actualPlayerAction</t>
+  </si>
+  <si>
+    <t>valeur stop de base</t>
+  </si>
+  <si>
+    <t>Change actualPlayerAction a play</t>
+  </si>
+  <si>
+    <t>Change actualPlayerAction a pause</t>
+  </si>
+  <si>
+    <t>Change actualPlayerAction a stop</t>
+  </si>
+  <si>
+    <t>previousCd</t>
+  </si>
+  <si>
+    <t>Int, contient l'id du CD si il y en a un sur le player (de 1 à 9, sauf 5 le lecteur)</t>
+  </si>
+  <si>
+    <t>Si la var previousCd est diffférente de 0, alors un CD est sur le lecteur</t>
+  </si>
+  <si>
+    <t>nextCd</t>
+  </si>
+  <si>
+    <t>On range le cd actuel a sa position</t>
+  </si>
+  <si>
+    <t>Prochain etat : wait</t>
+  </si>
+  <si>
+    <t>On se déplace en X et Y aux coordonnées coordGoTo</t>
+  </si>
+  <si>
+    <t>coordGoTo</t>
+  </si>
+  <si>
+    <t>Coordonnées ou doit se déplacer l'electroaimant</t>
+  </si>
+  <si>
+    <t>coordGoToAfter</t>
+  </si>
+  <si>
+    <t>Coordonnées ou doit se rendre l'elecroaimant ensuite (avant coordonnées ou prendre un cd, la ou poser)</t>
+  </si>
+  <si>
+    <t>On se déplace en X et Y aux coordonnées coordGoToAfter</t>
+  </si>
+  <si>
+    <t>Si enlever</t>
+  </si>
+  <si>
+    <t>GoToPos = 5 (position du lecteur)</t>
+  </si>
+  <si>
+    <t>GoToPosAfter = previousCd ( l'id du dernier cd poser sur le lecteur)</t>
+  </si>
+  <si>
+    <t>On récupère l'action voulu : placer un cd, enlever, wait</t>
+  </si>
+  <si>
+    <t>Si placer</t>
+  </si>
+  <si>
+    <t>Prochain etat : NewAction(wait)</t>
+  </si>
+  <si>
+    <t>Si wait</t>
+  </si>
+  <si>
+    <t>Prochain état : wait</t>
+  </si>
+  <si>
+    <t>GoToPos = previousCd, normalement init a l'ajout d'un cd</t>
+  </si>
+  <si>
+    <t>Si la var previousCD == 0</t>
+  </si>
+  <si>
+    <t>previousCd = nouvelle valeur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoToPosAfter = position du lecteur </t>
+  </si>
+  <si>
+    <t>nextCd est la position du lecteur</t>
+  </si>
+  <si>
+    <t>GoToPos = position previousCD</t>
+  </si>
+  <si>
+    <t>previousCd = 0</t>
+  </si>
+  <si>
+    <t>nextState</t>
+  </si>
+  <si>
+    <t>While nextStep null</t>
   </si>
 </sst>
 </file>
@@ -1226,7 +1409,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1263,8 +1446,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1421,11 +1616,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -1594,6 +1813,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1681,6 +1909,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1701,15 +1938,6 @@
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="2" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
@@ -1728,45 +1956,109 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>701040</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>531914</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>170105</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E9085EA-7110-1AD9-6D2B-D7606754ADD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7040880" y="0"/>
+          <a:ext cx="3000794" cy="4010585"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3E6AA73-8D41-471D-8991-A1E50578AF6D}" name="Tableau6" displayName="Tableau6" ref="C4:H64" totalsRowShown="0" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A3E6AA73-8D41-471D-8991-A1E50578AF6D}" name="Tableau6" displayName="Tableau6" ref="C4:H64" totalsRowShown="0" dataDxfId="30">
   <autoFilter ref="C4:H64" xr:uid="{A3E6AA73-8D41-471D-8991-A1E50578AF6D}"/>
   <tableColumns count="6">
-    <tableColumn id="11" xr3:uid="{C803E650-A104-4673-B4D1-0C8B2F2CCE65}" name="N° CDC" dataDxfId="26"/>
-    <tableColumn id="1" xr3:uid="{307B7E50-701C-4944-A12F-CBFB3F3AB728}" name="Tâche" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{0020EED0-8C09-4EF6-B338-1BC6FF444315}" name="Pré-condition" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{9113C3A7-3E6B-41D5-97A2-884C767BB0E0}" name="Matériel" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{8D213E42-5E00-4885-AD55-6F31956D6AFD}" name="Etat" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{F7E01085-CFB3-49DD-80E8-2936D707C247}" name="But" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{C803E650-A104-4673-B4D1-0C8B2F2CCE65}" name="N° CDC" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{307B7E50-701C-4944-A12F-CBFB3F3AB728}" name="Tâche" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{0020EED0-8C09-4EF6-B338-1BC6FF444315}" name="Pré-condition" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{9113C3A7-3E6B-41D5-97A2-884C767BB0E0}" name="Matériel" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{8D213E42-5E00-4885-AD55-6F31956D6AFD}" name="Etat" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{F7E01085-CFB3-49DD-80E8-2936D707C247}" name="But" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{64FBC46D-0810-4064-AFB4-A51FBFB88ADF}" name="Tableau7" displayName="Tableau7" ref="B5:D19" totalsRowShown="0">
-  <autoFilter ref="B5:D19" xr:uid="{64FBC46D-0810-4064-AFB4-A51FBFB88ADF}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{846AA218-6755-4F94-8080-5ED40BFBA0E7}" name="Init"/>
-    <tableColumn id="2" xr3:uid="{7F53351C-3C36-49BD-8E5C-A9B49AC57C6F}" name="GoToPos"/>
-    <tableColumn id="3" xr3:uid="{BB7ADEB9-1499-4F22-8285-A153989EA0E7}" name="Différentes fonctions"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{64FBC46D-0810-4064-AFB4-A51FBFB88ADF}" name="Tableau7" displayName="Tableau7" ref="E5:K28" totalsRowShown="0">
+  <autoFilter ref="E5:K28" xr:uid="{64FBC46D-0810-4064-AFB4-A51FBFB88ADF}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{846AA218-6755-4F94-8080-5ED40BFBA0E7}" name="GoToOrigin"/>
+    <tableColumn id="5" xr3:uid="{2662629C-D55D-4F52-A412-D3C790034197}" name="Wait"/>
+    <tableColumn id="2" xr3:uid="{7F53351C-3C36-49BD-8E5C-A9B49AC57C6F}" name="NewAction"/>
+    <tableColumn id="3" xr3:uid="{BB7ADEB9-1499-4F22-8285-A153989EA0E7}" name="GoToPos"/>
+    <tableColumn id="4" xr3:uid="{653A6A20-78CD-4C3F-888C-94284A724F8A}" name="Play"/>
+    <tableColumn id="6" xr3:uid="{BAAE1617-450B-40BD-AAFB-E2CFA79E5B03}" name="Pause"/>
+    <tableColumn id="7" xr3:uid="{128E5D0A-1410-41A0-AF95-5ECCB5252EA5}" name="Stop"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B23B5710-FFA6-411B-AC5C-7145D0E457FE}" name="Tableau2" displayName="Tableau2" ref="D4:E30" totalsRowShown="0" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{50606491-8634-4E27-A67D-91F7BB488A4D}" name="Tableau9" displayName="Tableau9" ref="A5:B16" totalsRowShown="0">
+  <autoFilter ref="A5:B16" xr:uid="{50606491-8634-4E27-A67D-91F7BB488A4D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{1F4C0D9B-4BD8-4E47-876E-6CDF3C064C39}" name="Variables"/>
+    <tableColumn id="2" xr3:uid="{7A056577-74C7-4A3A-B3DC-6ED3A8BB39E8}" name="Explocation"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B23B5710-FFA6-411B-AC5C-7145D0E457FE}" name="Tableau2" displayName="Tableau2" ref="D4:E30" totalsRowShown="0" dataDxfId="23">
   <autoFilter ref="D4:E30" xr:uid="{B23B5710-FFA6-411B-AC5C-7145D0E457FE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{14D3C3A4-AE5B-4AA1-9807-1A5CB1C24504}" name="Partie App" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{654FBC06-CD5D-446B-8DAE-0AF554F22DC1}" name="Priorité" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{14D3C3A4-AE5B-4AA1-9807-1A5CB1C24504}" name="Partie App" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{654FBC06-CD5D-446B-8DAE-0AF554F22DC1}" name="Priorité" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9417783B-493D-4582-A2AC-C62B5D9FD955}" name="Tableau3" displayName="Tableau3" ref="C39:F88" totalsRowShown="0">
   <autoFilter ref="C39:F88" xr:uid="{9417783B-493D-4582-A2AC-C62B5D9FD955}"/>
   <tableColumns count="4">
@@ -1779,7 +2071,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5AC7E31C-C286-4500-9C4E-317003642B50}" name="Tableau25" displayName="Tableau25" ref="C5:E32" totalsRowShown="0" dataDxfId="20">
   <autoFilter ref="C5:E32" xr:uid="{5AC7E31C-C286-4500-9C4E-317003642B50}"/>
   <tableColumns count="3">
@@ -1791,7 +2083,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DB3572F9-948B-46F3-B3B6-FEC25B584366}" name="Tableau36" displayName="Tableau36" ref="C35:E58" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="C35:E58" xr:uid="{DB3572F9-948B-46F3-B3B6-FEC25B584366}"/>
   <tableColumns count="3">
@@ -1803,7 +2095,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{50354B47-2411-4405-ADDE-4BB5CE46302B}" name="Tableau4" displayName="Tableau4" ref="C4:K30" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
   <autoFilter ref="C4:K30" xr:uid="{50354B47-2411-4405-ADDE-4BB5CE46302B}"/>
   <tableColumns count="9">
@@ -1821,7 +2113,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1676265-CD51-4C32-965D-94E769B5ABF3}" name="Tableau1" displayName="Tableau1" ref="C2:D11" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="C2:D11" xr:uid="{B1676265-CD51-4C32-965D-94E769B5ABF3}"/>
   <tableColumns count="2">
@@ -2129,56 +2421,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9697DB91-DDD7-46C2-9F18-DA7F9F25DA1F}">
-  <dimension ref="B3:C13"/>
+  <dimension ref="B3:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="F10" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+      <c r="N12" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>289</v>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2229,7 +2528,7 @@
   <dimension ref="C4:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2295,7 +2594,7 @@
         <v>201</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>205</v>
@@ -2309,7 +2608,7 @@
         <v>201</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>193</v>
@@ -2321,7 +2620,7 @@
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="19"/>
       <c r="D9" s="47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>193</v>
@@ -2333,10 +2632,10 @@
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="19"/>
       <c r="D10" s="47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F10" s="19"/>
       <c r="G10" s="45"/>
@@ -2345,10 +2644,10 @@
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="19"/>
       <c r="D11" s="44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F11" s="19"/>
       <c r="G11" s="69"/>
@@ -2357,7 +2656,7 @@
     <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="19"/>
       <c r="D12" s="47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -2367,7 +2666,7 @@
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="19"/>
       <c r="D13" s="47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -2377,7 +2676,7 @@
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="19"/>
       <c r="D14" s="47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
@@ -2387,10 +2686,10 @@
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="19"/>
       <c r="D15" s="44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F15" s="19"/>
       <c r="G15" s="69"/>
@@ -2399,7 +2698,7 @@
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="19"/>
       <c r="D16" s="47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
@@ -2417,10 +2716,10 @@
     <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="19"/>
       <c r="D18" s="46" t="s">
-        <v>206</v>
+        <v>300</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F18" s="19"/>
       <c r="G18" s="45"/>
@@ -2479,7 +2778,7 @@
         <v>152</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -2491,7 +2790,7 @@
         <v>152</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
@@ -2571,7 +2870,7 @@
         <v>167</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
@@ -2671,7 +2970,7 @@
         <v>155</v>
       </c>
       <c r="D40" s="44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
@@ -2683,10 +2982,10 @@
         <v>155</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="45"/>
@@ -2695,7 +2994,7 @@
     <row r="42" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C42" s="19"/>
       <c r="D42" s="44" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
@@ -2707,7 +3006,7 @@
         <v>157</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
@@ -2895,147 +3194,396 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91A8255-3274-4C2F-8C9A-BCAA8D10F9A8}">
-  <dimension ref="B5:H19"/>
+  <dimension ref="A5:K44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="69.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="111.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.21875" customWidth="1"/>
+    <col min="7" max="7" width="66" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="53" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.88671875" customWidth="1"/>
+    <col min="11" max="11" width="32.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>315</v>
+      </c>
       <c r="B5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="E5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F5" t="s">
+        <v>313</v>
+      </c>
+      <c r="G5" t="s">
+        <v>333</v>
+      </c>
+      <c r="H5" t="s">
         <v>282</v>
       </c>
-      <c r="C5" t="s">
-        <v>283</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
+        <v>334</v>
+      </c>
+      <c r="J5" t="s">
+        <v>335</v>
+      </c>
+      <c r="K5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="72" t="s">
+        <v>295</v>
+      </c>
+      <c r="E6" t="s">
         <v>310</v>
       </c>
-      <c r="H5" t="s">
+      <c r="F6" t="s">
+        <v>314</v>
+      </c>
+      <c r="G6" t="s">
+        <v>359</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="I6" t="s">
+        <v>341</v>
+      </c>
+      <c r="J6" t="s">
+        <v>342</v>
+      </c>
+      <c r="K6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>318</v>
+      </c>
+      <c r="F7" t="s">
+        <v>372</v>
+      </c>
+      <c r="G7" t="s">
+        <v>362</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="K7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D8" s="72" t="s">
+        <v>319</v>
+      </c>
+      <c r="G8" s="76" t="s">
+        <v>363</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D9" s="74" t="s">
+        <v>297</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>344</v>
+      </c>
+      <c r="B10" t="s">
+        <v>345</v>
+      </c>
+      <c r="D10" s="72"/>
+      <c r="G10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="s">
+        <v>352</v>
+      </c>
+      <c r="D11" s="74" t="s">
+        <v>296</v>
+      </c>
+      <c r="G11" s="76" t="s">
+        <v>357</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>353</v>
+      </c>
+      <c r="B12" t="s">
+        <v>354</v>
+      </c>
+      <c r="D12" s="72" t="s">
+        <v>320</v>
+      </c>
+      <c r="G12" s="76" t="s">
+        <v>358</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" t="s">
+        <v>324</v>
+      </c>
+      <c r="D13" s="74" t="s">
+        <v>321</v>
+      </c>
+      <c r="G13" s="76" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D14" s="72" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>337</v>
+      </c>
+      <c r="B15" t="s">
+        <v>338</v>
+      </c>
+      <c r="D15" s="74"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>339</v>
+      </c>
+      <c r="B16" t="s">
+        <v>340</v>
+      </c>
+      <c r="D16" s="72"/>
+      <c r="G16" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D17" s="74"/>
+      <c r="G17" s="76" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D18" s="72"/>
+      <c r="G18" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D19" s="74" t="s">
+        <v>311</v>
+      </c>
+      <c r="E19" t="s">
+        <v>312</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="H19" t="s">
+        <v>361</v>
+      </c>
+      <c r="I19" t="s">
+        <v>349</v>
+      </c>
+      <c r="J19" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D20" s="72"/>
+      <c r="G20" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D22" s="72"/>
+      <c r="G22" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G23" s="76"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="72"/>
+      <c r="G24" s="76" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D26" s="72"/>
+      <c r="G26" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G27" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D28" s="72"/>
+      <c r="G28" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D35" s="71" t="s">
+        <v>305</v>
+      </c>
+      <c r="E35" t="s">
+        <v>274</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D36" s="73" t="s">
+        <v>303</v>
+      </c>
+      <c r="E36" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>301</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F36" s="73" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D37" s="75" t="s">
+        <v>304</v>
+      </c>
+      <c r="E37" t="s">
+        <v>276</v>
+      </c>
+      <c r="F37" s="75" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D38" s="73" t="s">
+        <v>306</v>
+      </c>
+      <c r="E38" t="s">
+        <v>277</v>
+      </c>
+      <c r="F38" s="73" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D39" s="75" t="s">
+        <v>307</v>
+      </c>
+      <c r="E39" t="s">
+        <v>278</v>
+      </c>
+      <c r="F39" s="75" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E40" t="s">
+        <v>275</v>
+      </c>
+      <c r="F40" s="73" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E41" t="s">
+        <v>276</v>
+      </c>
+      <c r="F41" s="75" t="s">
         <v>294</v>
       </c>
-      <c r="H6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>303</v>
-      </c>
-      <c r="C7" t="s">
-        <v>295</v>
-      </c>
-      <c r="H7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>304</v>
-      </c>
-      <c r="C8" t="s">
-        <v>296</v>
-      </c>
-      <c r="H8" t="s">
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E42" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E43" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>305</v>
-      </c>
-      <c r="C9" t="s">
-        <v>297</v>
-      </c>
-      <c r="H9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>298</v>
-      </c>
-      <c r="H10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>302</v>
-      </c>
-      <c r="C11" t="s">
-        <v>299</v>
-      </c>
-      <c r="H11" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>306</v>
-      </c>
-      <c r="C12" t="s">
-        <v>300</v>
-      </c>
-      <c r="H12" t="s">
+    <row r="44" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E44" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>307</v>
-      </c>
-      <c r="H13" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>308</v>
-      </c>
-      <c r="H14" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>293</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3639,26 +4187,26 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" t="s">
         <v>230</v>
-      </c>
-      <c r="C4" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" t="s">
         <v>228</v>
-      </c>
-      <c r="C5" t="s">
-        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3882,7 +4430,7 @@
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -3896,7 +4444,7 @@
         <v>1</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="3:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3980,166 +4528,166 @@
     <row r="1" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="53" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="60" t="s">
         <v>235</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B5" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" s="50" t="s">
         <v>239</v>
-      </c>
-      <c r="C5" s="50" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B6" s="51"/>
       <c r="C6" s="52" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B7" s="51"/>
       <c r="C7" s="52" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B8" s="51"/>
       <c r="C8" s="52" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B9" s="51"/>
       <c r="C9" s="52" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B10" s="51"/>
       <c r="C10" s="52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B11" s="51"/>
       <c r="C11" s="52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B12" s="53"/>
       <c r="C12" s="54" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B13" s="59" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B14" s="48" t="s">
+        <v>251</v>
+      </c>
+      <c r="C14" s="55" t="s">
         <v>252</v>
-      </c>
-      <c r="C14" s="55" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B15" s="62" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" s="64"/>
       <c r="C16" s="65" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="64"/>
       <c r="C17" s="65" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="64"/>
       <c r="C18" s="65" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="64"/>
       <c r="C19" s="65" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="64"/>
       <c r="C20" s="65" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="64"/>
       <c r="C21" s="65" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="64"/>
       <c r="C22" s="65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="64"/>
       <c r="C23" s="65" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="64"/>
       <c r="C24" s="65" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="64"/>
       <c r="C25" s="65" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="64"/>
       <c r="C26" s="65" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
@@ -4149,33 +4697,33 @@
     <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="64"/>
       <c r="C28" s="65" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="64"/>
       <c r="C29" s="65" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="64"/>
       <c r="C30" s="65" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="64"/>
       <c r="C31" s="67" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="48" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C32" s="66" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On avance b encore. Mise en place d'attente quand on change de state, depuis flask. COmme ça on attend que la machine a é"tat fait son taff, avant de continuer cote flask. Amélioration du lien entre flask et machine, pour mise en palce d'un cd.
</commit_message>
<xml_diff>
--- a/NOUVEAU_Projet_Jukebox.xlsx
+++ b/NOUVEAU_Projet_Jukebox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Raspberry\Jukebox-V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6CCD4A-B983-4A90-815E-265FEFFDA32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8C2F15-73C9-4ECD-B7AA-B5712620B44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taches en cours" sheetId="12" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="374">
   <si>
     <t>Partie App</t>
   </si>
@@ -1318,6 +1318,9 @@
   </si>
   <si>
     <t>While nextStep null</t>
+  </si>
+  <si>
+    <t>detecter la fin de course d el'qimant en z</t>
   </si>
 </sst>
 </file>
@@ -2423,8 +2426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9697DB91-DDD7-46C2-9F18-DA7F9F25DA1F}">
   <dimension ref="B3:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2468,6 +2471,11 @@
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
@@ -3196,7 +3204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F91A8255-3274-4C2F-8C9A-BCAA8D10F9A8}">
   <dimension ref="A5:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>